<commit_message>
stroke units luxembourg gps data
</commit_message>
<xml_diff>
--- a/daten/stroke_units_lu.xlsx
+++ b/daten/stroke_units_lu.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3a87f39a522517ac/FHGR/4. Semester/Masterthesis/Daten/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurazanchin/Dropbox/Mac/Desktop/master/daten/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5151986D-BE26-A341-8255-3CFF227E1889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A77DC2-C8E0-644D-90D4-F076D74DD2F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="2600" windowWidth="27440" windowHeight="16240" xr2:uid="{703E470E-EBFD-0D4E-94A4-7298E40D5768}"/>
+    <workbookView xWindow="6160" yWindow="2880" windowWidth="27440" windowHeight="16240" xr2:uid="{703E470E-EBFD-0D4E-94A4-7298E40D5768}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Klinik</t>
   </si>
@@ -50,12 +50,6 @@
     <t>Ort</t>
   </si>
   <si>
-    <t>Anzahl</t>
-  </si>
-  <si>
-    <t>Stroke Units Luxemburg</t>
-  </si>
-  <si>
     <t>Centre hospitalier de Luxembourg</t>
   </si>
   <si>
@@ -71,18 +65,12 @@
     <t>Neudorf-Weimershof</t>
   </si>
   <si>
-    <t>Emile Mayrisch Street</t>
-  </si>
-  <si>
     <t>Esch-sur-Alzette</t>
   </si>
   <si>
     <t>Ettelbruck</t>
   </si>
   <si>
-    <t>Rollengergronn-Belair-Nord</t>
-  </si>
-  <si>
     <t>Rue Nicolas Ernest Barblé 4</t>
   </si>
   <si>
@@ -90,6 +78,12 @@
   </si>
   <si>
     <t>Rue Edward Steichen 9</t>
+  </si>
+  <si>
+    <t>Rue Emile Mayrisch</t>
+  </si>
+  <si>
+    <t>Luxembourg</t>
   </si>
 </sst>
 </file>
@@ -105,10 +99,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -149,10 +145,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -452,112 +444,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA90C6D4-C3FC-C54A-AA8E-1FD120BC0EAE}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" customWidth="1"/>
-    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2">
+        <v>1210</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3">
+        <v>4240</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>3</v>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>9080</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4">
-        <v>1210</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>2</v>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5">
-        <v>4240</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>2540</v>
+      </c>
+      <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6">
-        <v>9080</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7">
-        <v>2540</v>
-      </c>
-      <c r="E7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>